<commit_message>
add sign-seal part and vurse
</commit_message>
<xml_diff>
--- a/files/sum up f es/Electronic-Seal-Struct-Rules.xlsx
+++ b/files/sum up f es/Electronic-Seal-Struct-Rules.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAE8C33-45D8-438A-A411-00BBCC82AECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11316" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="结构对比" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="88">
   <si>
     <t>IA5String</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -335,13 +334,49 @@
   </si>
   <si>
     <t>BIT STRING OPTIONAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>签名算法标识:signatureAlgorithm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>签章人证书和算法标识在二级结构中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>签章人证书和算法标识调到一级结构中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无时间戳可选项结构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一级结构中增加了时间戳可选项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电子签章结构对比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待签名数据的内容发生项目增减</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GMT 0031-2014 安全电子签章密码技术规范</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GUOBAN-电子公文体系：安全电子签章密码技术规范</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -635,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -730,16 +765,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -781,47 +867,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -841,7 +894,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -916,23 +969,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -968,23 +1004,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1160,22 +1179,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.125" customWidth="1"/>
-    <col min="3" max="3" width="46.5" customWidth="1"/>
-    <col min="4" max="4" width="41.5" customWidth="1"/>
-    <col min="5" max="5" width="37.125" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" customWidth="1"/>
+    <col min="3" max="3" width="46.44140625" customWidth="1"/>
+    <col min="4" max="4" width="41.44140625" customWidth="1"/>
+    <col min="5" max="5" width="37.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
         <v>56</v>
@@ -1187,8 +1206,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="27" x14ac:dyDescent="0.15">
-      <c r="B3" s="32" t="s">
+    <row r="3" spans="2:5" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B3" s="45" t="s">
         <v>62</v>
       </c>
       <c r="C3" s="31" t="s">
@@ -1201,8 +1220,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B4" s="32"/>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="45"/>
       <c r="C4" t="s">
         <v>63</v>
       </c>
@@ -1210,12 +1229,36 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B5" s="32"/>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="45"/>
+    </row>
+    <row r="8" spans="2:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="45"/>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1224,34 +1267,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:H40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="1"/>
-    <col min="2" max="2" width="3.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="32.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="3.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="32.109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="32" style="1" customWidth="1"/>
-    <col min="8" max="8" width="33.5" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.875" style="1"/>
+    <col min="8" max="8" width="33.44140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B3" s="38" t="s">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+    </row>
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="47" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -1263,10 +1317,10 @@
       <c r="G3" s="14"/>
       <c r="H3" s="15"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B4" s="39"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="56"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1276,10 +1330,10 @@
       <c r="G4" s="11"/>
       <c r="H4" s="16"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B5" s="39"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="56"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
       <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1289,9 +1343,9 @@
       <c r="G5" s="11"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B6" s="39"/>
-      <c r="C6" s="35"/>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="56"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1302,10 +1356,10 @@
       <c r="G6" s="11"/>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B7" s="39"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="41" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="56"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="58" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -1317,10 +1371,10 @@
       <c r="G7" s="11"/>
       <c r="H7" s="16"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B8" s="39"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="41"/>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="56"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="58"/>
       <c r="E8" s="9" t="s">
         <v>12</v>
       </c>
@@ -1330,10 +1384,10 @@
       <c r="G8" s="11"/>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B9" s="39"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="41"/>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="56"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="58"/>
       <c r="E9" s="8" t="s">
         <v>13</v>
       </c>
@@ -1343,11 +1397,11 @@
       <c r="G9" s="11"/>
       <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B10" s="39"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="42" t="s">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="56"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="59" t="s">
         <v>45</v>
       </c>
       <c r="F10" s="10" t="s">
@@ -1360,36 +1414,36 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="39"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="37" t="s">
+    <row r="11" spans="2:8" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="56"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="53" t="s">
         <v>30</v>
       </c>
       <c r="H11" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="39"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="36"/>
+    <row r="12" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="56"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="53"/>
       <c r="H12" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B13" s="39"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="41"/>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="56"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="58"/>
       <c r="E13" s="12" t="s">
         <v>21</v>
       </c>
@@ -1399,10 +1453,10 @@
       <c r="G13" s="20"/>
       <c r="H13" s="16"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B14" s="39"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="41"/>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="56"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="58"/>
       <c r="E14" s="10" t="s">
         <v>22</v>
       </c>
@@ -1412,10 +1466,10 @@
       <c r="G14" s="20"/>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B15" s="39"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="41"/>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="56"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="58"/>
       <c r="E15" s="3" t="s">
         <v>23</v>
       </c>
@@ -1425,10 +1479,10 @@
       <c r="G15" s="20"/>
       <c r="H15" s="16"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B16" s="39"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="44" t="s">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="56"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="61" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -1440,10 +1494,10 @@
       <c r="G16" s="2"/>
       <c r="H16" s="16"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B17" s="39"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="44"/>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="56"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="61"/>
       <c r="E17" s="9" t="s">
         <v>34</v>
       </c>
@@ -1453,10 +1507,10 @@
       <c r="G17" s="2"/>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B18" s="39"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="44"/>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="56"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="61"/>
       <c r="E18" s="8" t="s">
         <v>35</v>
       </c>
@@ -1466,10 +1520,10 @@
       <c r="G18" s="2"/>
       <c r="H18" s="21"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B19" s="39"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="44"/>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="56"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="61"/>
       <c r="E19" s="12" t="s">
         <v>36</v>
       </c>
@@ -1479,10 +1533,10 @@
       <c r="G19" s="2"/>
       <c r="H19" s="16"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="39"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="33" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="56"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="52" t="s">
         <v>76</v>
       </c>
       <c r="E20" s="10" t="s">
@@ -1494,10 +1548,10 @@
       <c r="G20" s="2"/>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="39"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="33"/>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="56"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="52"/>
       <c r="E21" s="3" t="s">
         <v>38</v>
       </c>
@@ -1507,10 +1561,10 @@
       <c r="G21" s="2"/>
       <c r="H21" s="16"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="39"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="33"/>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="56"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="52"/>
       <c r="E22" s="4" t="s">
         <v>39</v>
       </c>
@@ -1520,8 +1574,8 @@
       <c r="G22" s="2"/>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="39"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="56"/>
       <c r="C23" s="3" t="s">
         <v>17</v>
       </c>
@@ -1533,8 +1587,8 @@
       <c r="G23" s="2"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="39"/>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="56"/>
       <c r="C24" s="4" t="s">
         <v>18</v>
       </c>
@@ -1546,8 +1600,8 @@
       <c r="G24" s="2"/>
       <c r="H24" s="16"/>
     </row>
-    <row r="25" spans="2:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="40"/>
+    <row r="25" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="57"/>
       <c r="C25" s="22" t="s">
         <v>19</v>
       </c>
@@ -1559,70 +1613,70 @@
       <c r="G25" s="23"/>
       <c r="H25" s="24"/>
     </row>
-    <row r="28" spans="2:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="55" t="s">
+      <c r="D29" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="E29" s="55" t="s">
+      <c r="E29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="F29" s="50"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B30" s="51"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="56" t="s">
+      <c r="F29" s="35"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="50"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="E30" s="56" t="s">
+      <c r="E30" s="39" t="s">
         <v>72</v>
       </c>
       <c r="F30" s="21"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B31" s="51"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="57" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="50"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="E31" s="57" t="s">
+      <c r="E31" s="40" t="s">
         <v>24</v>
       </c>
       <c r="F31" s="21"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B32" s="51"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="58" t="s">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="50"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="58" t="s">
+      <c r="E32" s="41" t="s">
         <v>44</v>
       </c>
       <c r="F32" s="21"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B33" s="51"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="59" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="50"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="E33" s="59" t="s">
+      <c r="E33" s="42" t="s">
         <v>0</v>
       </c>
       <c r="F33" s="21"/>
     </row>
-    <row r="34" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="51"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="60" t="s">
+    <row r="34" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="50"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="46" t="s">
         <v>76</v>
       </c>
       <c r="E34" s="10" t="s">
@@ -1632,10 +1686,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B35" s="51"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="60"/>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="50"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="46"/>
       <c r="E35" s="6" t="s">
         <v>38</v>
       </c>
@@ -1643,10 +1697,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B36" s="51"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="60"/>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="50"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="46"/>
       <c r="E36" s="7" t="s">
         <v>39</v>
       </c>
@@ -1654,57 +1708,53 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B37" s="51"/>
-      <c r="C37" s="61" t="s">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="50"/>
+      <c r="C37" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="D37" s="61" t="s">
+      <c r="D37" s="43" t="s">
         <v>32</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="21"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B38" s="51"/>
-      <c r="C38" s="56" t="s">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="50"/>
+      <c r="C38" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="D38" s="56" t="s">
+      <c r="D38" s="39" t="s">
         <v>40</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="21"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B39" s="51"/>
-      <c r="C39" s="57" t="s">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="50"/>
+      <c r="C39" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="D39" s="57" t="s">
+      <c r="D39" s="40" t="s">
         <v>44</v>
       </c>
       <c r="E39" s="11"/>
       <c r="F39" s="21"/>
     </row>
-    <row r="40" spans="2:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="52"/>
-      <c r="C40" s="62" t="s">
+    <row r="40" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="51"/>
+      <c r="C40" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="D40" s="62" t="s">
+      <c r="D40" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="53"/>
-      <c r="F40" s="54"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="C29:C36"/>
-    <mergeCell ref="B29:B40"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="C3:C22"/>
+  <mergeCells count="13">
+    <mergeCell ref="B1:H1"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="B3:B25"/>
@@ -1712,6 +1762,11 @@
     <mergeCell ref="D7:D15"/>
     <mergeCell ref="E10:E12"/>
     <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="C29:C36"/>
+    <mergeCell ref="B29:B40"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="C3:C22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1719,31 +1774,40 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:F22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.25" customWidth="1"/>
-    <col min="3" max="3" width="28.5" customWidth="1"/>
-    <col min="4" max="4" width="27.875" customWidth="1"/>
-    <col min="5" max="5" width="43.5" customWidth="1"/>
-    <col min="6" max="6" width="32.125" customWidth="1"/>
+    <col min="2" max="2" width="3.21875" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" customWidth="1"/>
+    <col min="4" max="4" width="31.77734375" customWidth="1"/>
+    <col min="5" max="5" width="43.44140625" customWidth="1"/>
+    <col min="6" max="6" width="32.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B3" s="38" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+    </row>
+    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="47" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -1753,10 +1817,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B4" s="39"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="56"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1764,10 +1828,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B5" s="39"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="56"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
       <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1775,9 +1839,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B6" s="39"/>
-      <c r="C6" s="35"/>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="56"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1786,10 +1850,10 @@
       </c>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B7" s="39"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="41" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="56"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="58" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -1799,10 +1863,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B8" s="39"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="41"/>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="56"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="58"/>
       <c r="E8" s="9" t="s">
         <v>12</v>
       </c>
@@ -1810,10 +1874,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="39"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="41"/>
+    <row r="9" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="56"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="58"/>
       <c r="E9" s="25" t="s">
         <v>53</v>
       </c>
@@ -1821,10 +1885,10 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B10" s="39"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="41"/>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="56"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="58"/>
       <c r="E10" s="12" t="s">
         <v>21</v>
       </c>
@@ -1832,10 +1896,10 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B11" s="39"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="41"/>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="56"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="58"/>
       <c r="E11" s="10" t="s">
         <v>22</v>
       </c>
@@ -1843,10 +1907,10 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B12" s="39"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="41"/>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="56"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="58"/>
       <c r="E12" s="3" t="s">
         <v>23</v>
       </c>
@@ -1854,10 +1918,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B13" s="39"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="44" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="56"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="61" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -1867,10 +1931,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B14" s="39"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="44"/>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="56"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="61"/>
       <c r="E14" s="9" t="s">
         <v>34</v>
       </c>
@@ -1878,10 +1942,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B15" s="39"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="44"/>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="56"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="61"/>
       <c r="E15" s="8" t="s">
         <v>35</v>
       </c>
@@ -1889,10 +1953,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B16" s="39"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="44"/>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="56"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="61"/>
       <c r="E16" s="12" t="s">
         <v>36</v>
       </c>
@@ -1900,10 +1964,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B17" s="39"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="45" t="s">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="56"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="62" t="s">
         <v>50</v>
       </c>
       <c r="E17" s="10" t="s">
@@ -1913,10 +1977,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B18" s="39"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="33"/>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="56"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="52"/>
       <c r="E18" s="3" t="s">
         <v>38</v>
       </c>
@@ -1924,10 +1988,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B19" s="39"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="33"/>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="56"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="52"/>
       <c r="E19" s="4" t="s">
         <v>39</v>
       </c>
@@ -1935,9 +1999,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B20" s="39"/>
-      <c r="C20" s="46" t="s">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="56"/>
+      <c r="C20" s="63" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -1948,9 +2012,9 @@
       </c>
       <c r="F20" s="16"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B21" s="39"/>
-      <c r="C21" s="47"/>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="56"/>
+      <c r="C21" s="64"/>
       <c r="D21" s="4" t="s">
         <v>18</v>
       </c>
@@ -1959,9 +2023,9 @@
       </c>
       <c r="F21" s="16"/>
     </row>
-    <row r="22" spans="2:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="40"/>
-      <c r="C22" s="48"/>
+    <row r="22" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="57"/>
+      <c r="C22" s="65"/>
       <c r="D22" s="22" t="s">
         <v>55</v>
       </c>
@@ -1970,8 +2034,140 @@
       </c>
       <c r="F22" s="24"/>
     </row>
+    <row r="26" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="35"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="50"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" s="21"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="50"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="21"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="50"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="21"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="50"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" s="21"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="50"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="50"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="50"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="50"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" s="21"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="50"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="21"/>
+    </row>
+    <row r="37" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="51"/>
+      <c r="C37" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="36"/>
+      <c r="F37" s="37"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="11">
+    <mergeCell ref="B27:B37"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="C27:C36"/>
+    <mergeCell ref="B1:F1"/>
     <mergeCell ref="D13:D16"/>
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="C20:C22"/>

</xml_diff>

<commit_message>
add eseal-rule on GBT-38540
</commit_message>
<xml_diff>
--- a/files/sum up f es/Electronic-Seal-Struct-Rules.xlsx
+++ b/files/sum up f es/Electronic-Seal-Struct-Rules.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11316" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11316" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="结构对比" sheetId="1" r:id="rId1"/>
     <sheet name="GUOBAN标准" sheetId="3" r:id="rId2"/>
     <sheet name="GMT-0031标准" sheetId="2" r:id="rId3"/>
+    <sheet name="GBT38540-2020" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="96">
   <si>
     <t>IA5String</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -370,6 +371,38 @@
   </si>
   <si>
     <t>GUOBAN-电子公文体系：安全电子签章密码技术规范</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GB/T 38540-2020 ：信息安全计算 安全电子签章密码技术规范</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本版为4， 表示v4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>签章人证书信息类型:certListType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-数字证书，22=数字证书对应的杂凑值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位毫米mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GIF,BMP,JPG,PNG,SVG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>与电子印章版本一致，本标准为4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>der编码的r，s 序列， 即pkcs1签名结构</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -670,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -804,18 +837,72 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -828,32 +915,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -865,15 +928,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1207,7 +1261,7 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="53" t="s">
         <v>62</v>
       </c>
       <c r="C3" s="31" t="s">
@@ -1221,7 +1275,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="45"/>
+      <c r="B4" s="53"/>
       <c r="C4" t="s">
         <v>63</v>
       </c>
@@ -1230,10 +1284,10 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="45"/>
+      <c r="B5" s="53"/>
     </row>
     <row r="8" spans="2:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="53" t="s">
         <v>84</v>
       </c>
       <c r="C8" t="s">
@@ -1247,7 +1301,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="45"/>
+      <c r="B9" s="53"/>
       <c r="C9" t="s">
         <v>82</v>
       </c>
@@ -1270,7 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:H1"/>
     </sheetView>
   </sheetViews>
@@ -1287,25 +1341,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="60" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -1318,9 +1372,9 @@
       <c r="H3" s="15"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="56"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
       <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1331,9 +1385,9 @@
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="56"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
       <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1344,8 +1398,8 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="56"/>
-      <c r="C6" s="48"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1357,9 +1411,9 @@
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="56"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="58" t="s">
+      <c r="B7" s="58"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="62" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -1372,9 +1426,9 @@
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="56"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="58"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="62"/>
       <c r="E8" s="9" t="s">
         <v>12</v>
       </c>
@@ -1385,9 +1439,9 @@
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="56"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="58"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="62"/>
       <c r="E9" s="8" t="s">
         <v>13</v>
       </c>
@@ -1398,10 +1452,10 @@
       <c r="H9" s="16"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="56"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59" t="s">
+      <c r="B10" s="58"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="63" t="s">
         <v>45</v>
       </c>
       <c r="F10" s="10" t="s">
@@ -1415,14 +1469,14 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="56"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="54" t="s">
+      <c r="B11" s="58"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="53" t="s">
+      <c r="G11" s="55" t="s">
         <v>30</v>
       </c>
       <c r="H11" s="18" t="s">
@@ -1430,20 +1484,20 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="56"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="53"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="55"/>
       <c r="H12" s="19" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="56"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="58"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="62"/>
       <c r="E13" s="12" t="s">
         <v>21</v>
       </c>
@@ -1454,9 +1508,9 @@
       <c r="H13" s="16"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="56"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="58"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="62"/>
       <c r="E14" s="10" t="s">
         <v>22</v>
       </c>
@@ -1467,9 +1521,9 @@
       <c r="H14" s="16"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="56"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="58"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="62"/>
       <c r="E15" s="3" t="s">
         <v>23</v>
       </c>
@@ -1480,9 +1534,9 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="56"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="61" t="s">
+      <c r="B16" s="58"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="65" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -1495,9 +1549,9 @@
       <c r="H16" s="16"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="56"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="61"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="65"/>
       <c r="E17" s="9" t="s">
         <v>34</v>
       </c>
@@ -1508,9 +1562,9 @@
       <c r="H17" s="16"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="56"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="61"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="65"/>
       <c r="E18" s="8" t="s">
         <v>35</v>
       </c>
@@ -1521,9 +1575,9 @@
       <c r="H18" s="21"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="56"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="61"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="65"/>
       <c r="E19" s="12" t="s">
         <v>36</v>
       </c>
@@ -1534,9 +1588,9 @@
       <c r="H19" s="16"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="56"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="52" t="s">
+      <c r="B20" s="58"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="70" t="s">
         <v>76</v>
       </c>
       <c r="E20" s="10" t="s">
@@ -1549,9 +1603,9 @@
       <c r="H20" s="16"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="56"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="52"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="70"/>
       <c r="E21" s="3" t="s">
         <v>38</v>
       </c>
@@ -1562,9 +1616,9 @@
       <c r="H21" s="16"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="56"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="52"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="70"/>
       <c r="E22" s="4" t="s">
         <v>39</v>
       </c>
@@ -1575,7 +1629,7 @@
       <c r="H22" s="16"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="56"/>
+      <c r="B23" s="58"/>
       <c r="C23" s="3" t="s">
         <v>17</v>
       </c>
@@ -1588,7 +1642,7 @@
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="56"/>
+      <c r="B24" s="58"/>
       <c r="C24" s="4" t="s">
         <v>18</v>
       </c>
@@ -1601,7 +1655,7 @@
       <c r="H24" s="16"/>
     </row>
     <row r="25" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="57"/>
+      <c r="B25" s="59"/>
       <c r="C25" s="22" t="s">
         <v>19</v>
       </c>
@@ -1615,10 +1669,10 @@
     </row>
     <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="47" t="s">
+      <c r="C29" s="60" t="s">
         <v>65</v>
       </c>
       <c r="D29" s="38" t="s">
@@ -1630,8 +1684,8 @@
       <c r="F29" s="35"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="50"/>
-      <c r="C30" s="48"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="39" t="s">
         <v>71</v>
       </c>
@@ -1641,8 +1695,8 @@
       <c r="F30" s="21"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="50"/>
-      <c r="C31" s="48"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="40" t="s">
         <v>73</v>
       </c>
@@ -1652,8 +1706,8 @@
       <c r="F31" s="21"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="50"/>
-      <c r="C32" s="48"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="41" t="s">
         <v>74</v>
       </c>
@@ -1663,8 +1717,8 @@
       <c r="F32" s="21"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="50"/>
-      <c r="C33" s="48"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="61"/>
       <c r="D33" s="42" t="s">
         <v>75</v>
       </c>
@@ -1674,9 +1728,9 @@
       <c r="F33" s="21"/>
     </row>
     <row r="34" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="50"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="46" t="s">
+      <c r="B34" s="68"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="66" t="s">
         <v>76</v>
       </c>
       <c r="E34" s="10" t="s">
@@ -1687,9 +1741,9 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="50"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="46"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="66"/>
       <c r="E35" s="6" t="s">
         <v>38</v>
       </c>
@@ -1698,9 +1752,9 @@
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="50"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="46"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="66"/>
       <c r="E36" s="7" t="s">
         <v>39</v>
       </c>
@@ -1709,7 +1763,7 @@
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="50"/>
+      <c r="B37" s="68"/>
       <c r="C37" s="43" t="s">
         <v>66</v>
       </c>
@@ -1720,7 +1774,7 @@
       <c r="F37" s="21"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="50"/>
+      <c r="B38" s="68"/>
       <c r="C38" s="39" t="s">
         <v>67</v>
       </c>
@@ -1731,7 +1785,7 @@
       <c r="F38" s="21"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="50"/>
+      <c r="B39" s="68"/>
       <c r="C39" s="40" t="s">
         <v>68</v>
       </c>
@@ -1742,7 +1796,7 @@
       <c r="F39" s="21"/>
     </row>
     <row r="40" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="51"/>
+      <c r="B40" s="69"/>
       <c r="C40" s="44" t="s">
         <v>69</v>
       </c>
@@ -1754,6 +1808,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="C29:C36"/>
+    <mergeCell ref="B29:B40"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="C3:C22"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="F11:F12"/>
@@ -1762,11 +1821,6 @@
     <mergeCell ref="D7:D15"/>
     <mergeCell ref="E10:E12"/>
     <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="C29:C36"/>
-    <mergeCell ref="B29:B40"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="C3:C22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1777,7 +1831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
@@ -1791,23 +1845,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
     </row>
     <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="60" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -1818,9 +1872,9 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="56"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
       <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1829,9 +1883,9 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="56"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
       <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1840,8 +1894,8 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="56"/>
-      <c r="C6" s="48"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1851,9 +1905,9 @@
       <c r="F6" s="16"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="56"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="58" t="s">
+      <c r="B7" s="58"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="62" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -1864,9 +1918,9 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="56"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="58"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="62"/>
       <c r="E8" s="9" t="s">
         <v>12</v>
       </c>
@@ -1875,9 +1929,9 @@
       </c>
     </row>
     <row r="9" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="56"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="58"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="62"/>
       <c r="E9" s="25" t="s">
         <v>53</v>
       </c>
@@ -1886,9 +1940,9 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="56"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="58"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="62"/>
       <c r="E10" s="12" t="s">
         <v>21</v>
       </c>
@@ -1897,9 +1951,9 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="56"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="58"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="62"/>
       <c r="E11" s="10" t="s">
         <v>22</v>
       </c>
@@ -1908,9 +1962,9 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="56"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="58"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="62"/>
       <c r="E12" s="3" t="s">
         <v>23</v>
       </c>
@@ -1919,9 +1973,9 @@
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="56"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="61" t="s">
+      <c r="B13" s="58"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="65" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -1932,9 +1986,9 @@
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="56"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="61"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="65"/>
       <c r="E14" s="9" t="s">
         <v>34</v>
       </c>
@@ -1943,9 +1997,9 @@
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="56"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="61"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="65"/>
       <c r="E15" s="8" t="s">
         <v>35</v>
       </c>
@@ -1954,9 +2008,9 @@
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="56"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="61"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="65"/>
       <c r="E16" s="12" t="s">
         <v>36</v>
       </c>
@@ -1965,9 +2019,9 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="56"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="62" t="s">
+      <c r="B17" s="58"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="72" t="s">
         <v>50</v>
       </c>
       <c r="E17" s="10" t="s">
@@ -1978,9 +2032,9 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="56"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="52"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="70"/>
       <c r="E18" s="3" t="s">
         <v>38</v>
       </c>
@@ -1989,9 +2043,9 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="56"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="52"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="70"/>
       <c r="E19" s="4" t="s">
         <v>39</v>
       </c>
@@ -2000,8 +2054,8 @@
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="56"/>
-      <c r="C20" s="63" t="s">
+      <c r="B20" s="58"/>
+      <c r="C20" s="73" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -2013,8 +2067,8 @@
       <c r="F20" s="16"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="56"/>
-      <c r="C21" s="64"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="74"/>
       <c r="D21" s="4" t="s">
         <v>18</v>
       </c>
@@ -2024,8 +2078,8 @@
       <c r="F21" s="16"/>
     </row>
     <row r="22" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="57"/>
-      <c r="C22" s="65"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="75"/>
       <c r="D22" s="22" t="s">
         <v>55</v>
       </c>
@@ -2036,10 +2090,10 @@
     </row>
     <row r="26" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="60" t="s">
         <v>65</v>
       </c>
       <c r="D27" s="38" t="s">
@@ -2051,8 +2105,8 @@
       <c r="F27" s="35"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="50"/>
-      <c r="C28" s="48"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="39" t="s">
         <v>71</v>
       </c>
@@ -2062,8 +2116,8 @@
       <c r="F28" s="21"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="50"/>
-      <c r="C29" s="48"/>
+      <c r="B29" s="68"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="40" t="s">
         <v>73</v>
       </c>
@@ -2073,8 +2127,8 @@
       <c r="F29" s="21"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="50"/>
-      <c r="C30" s="48"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="41" t="s">
         <v>74</v>
       </c>
@@ -2084,8 +2138,8 @@
       <c r="F30" s="21"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="50"/>
-      <c r="C31" s="48"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="42" t="s">
         <v>75</v>
       </c>
@@ -2095,9 +2149,9 @@
       <c r="F31" s="21"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="50"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="46" t="s">
+      <c r="B32" s="68"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="66" t="s">
         <v>76</v>
       </c>
       <c r="E32" s="32" t="s">
@@ -2108,9 +2162,9 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="50"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="46"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="66"/>
       <c r="E33" s="33" t="s">
         <v>38</v>
       </c>
@@ -2119,9 +2173,9 @@
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="50"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="46"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="66"/>
       <c r="E34" s="34" t="s">
         <v>39</v>
       </c>
@@ -2130,8 +2184,8 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="50"/>
-      <c r="C35" s="48"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="61"/>
       <c r="D35" s="43" t="s">
         <v>66</v>
       </c>
@@ -2141,8 +2195,8 @@
       <c r="F35" s="21"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="50"/>
-      <c r="C36" s="48"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="61"/>
       <c r="D36" s="39" t="s">
         <v>79</v>
       </c>
@@ -2152,11 +2206,11 @@
       <c r="F36" s="21"/>
     </row>
     <row r="37" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="51"/>
-      <c r="C37" s="66" t="s">
+      <c r="B37" s="69"/>
+      <c r="C37" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="66" t="s">
+      <c r="D37" s="51" t="s">
         <v>44</v>
       </c>
       <c r="E37" s="36"/>
@@ -2179,4 +2233,552 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="52"/>
+    <col min="2" max="2" width="3.21875" style="52" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" style="52" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" style="52" customWidth="1"/>
+    <col min="5" max="6" width="32.109375" style="52" customWidth="1"/>
+    <col min="7" max="7" width="32" style="52" customWidth="1"/>
+    <col min="8" max="8" width="33.44140625" style="52" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="52"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+    </row>
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="58"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="58"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="58"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="58"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="58"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="58"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="58"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="58"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="58"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="58"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="58"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="20"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="58"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="58"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="58"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="58"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="21"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="58"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="58"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="58"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="16"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="58"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="58"/>
+      <c r="C23" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="16"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="58"/>
+      <c r="C24" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="16"/>
+    </row>
+    <row r="25" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="59"/>
+      <c r="C25" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="H25" s="24"/>
+    </row>
+    <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H29" s="35"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="68"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="21"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="68"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="21"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="68"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="21"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="68"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="21"/>
+    </row>
+    <row r="34" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="68"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="66" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" s="11"/>
+      <c r="H34" s="21"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="68"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="G35" s="11"/>
+      <c r="H35" s="21"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="68"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" s="11"/>
+      <c r="H36" s="21"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="68"/>
+      <c r="C37" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="21"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="68"/>
+      <c r="C38" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="21"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="68"/>
+      <c r="C39" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H39" s="21"/>
+    </row>
+    <row r="40" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="69"/>
+      <c r="C40" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="B29:B40"/>
+    <mergeCell ref="C29:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:B25"/>
+    <mergeCell ref="C3:C22"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="D7:D15"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D20:D22"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add all in dir
</commit_message>
<xml_diff>
--- a/files/sum up f es/Electronic-Seal-Struct-Rules.xlsx
+++ b/files/sum up f es/Electronic-Seal-Struct-Rules.xlsx
@@ -386,10 +386,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1-数字证书，22=数字证书对应的杂凑值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>单位毫米mm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -403,6 +399,10 @@
   </si>
   <si>
     <t>der编码的r，s 序列， 即pkcs1签名结构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-数字证书，2=数字证书对应的杂凑值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -864,6 +864,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -882,12 +903,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -898,21 +913,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1341,25 +1341,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
     </row>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="55" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -1372,9 +1372,9 @@
       <c r="H3" s="15"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="58"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1385,9 +1385,9 @@
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="58"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1398,8 +1398,8 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="58"/>
-      <c r="C6" s="61"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1411,9 +1411,9 @@
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="58"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="62" t="s">
+      <c r="B7" s="65"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="67" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -1426,9 +1426,9 @@
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="58"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="62"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="67"/>
       <c r="E8" s="9" t="s">
         <v>12</v>
       </c>
@@ -1439,9 +1439,9 @@
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="58"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="62"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="67"/>
       <c r="E9" s="8" t="s">
         <v>13</v>
       </c>
@@ -1452,10 +1452,10 @@
       <c r="H9" s="16"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="58"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="63" t="s">
+      <c r="B10" s="65"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="68" t="s">
         <v>45</v>
       </c>
       <c r="F10" s="10" t="s">
@@ -1469,14 +1469,14 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="58"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="56" t="s">
+      <c r="B11" s="65"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="55" t="s">
+      <c r="G11" s="62" t="s">
         <v>30</v>
       </c>
       <c r="H11" s="18" t="s">
@@ -1484,20 +1484,20 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="58"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="55"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="62"/>
       <c r="H12" s="19" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="58"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="62"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="67"/>
       <c r="E13" s="12" t="s">
         <v>21</v>
       </c>
@@ -1508,9 +1508,9 @@
       <c r="H13" s="16"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="58"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="62"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="67"/>
       <c r="E14" s="10" t="s">
         <v>22</v>
       </c>
@@ -1521,9 +1521,9 @@
       <c r="H14" s="16"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="58"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="62"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="67"/>
       <c r="E15" s="3" t="s">
         <v>23</v>
       </c>
@@ -1534,9 +1534,9 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="58"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="65" t="s">
+      <c r="B16" s="65"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="70" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -1549,9 +1549,9 @@
       <c r="H16" s="16"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="58"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="65"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="70"/>
       <c r="E17" s="9" t="s">
         <v>34</v>
       </c>
@@ -1562,9 +1562,9 @@
       <c r="H17" s="16"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="58"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="65"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="70"/>
       <c r="E18" s="8" t="s">
         <v>35</v>
       </c>
@@ -1575,9 +1575,9 @@
       <c r="H18" s="21"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="58"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="65"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="70"/>
       <c r="E19" s="12" t="s">
         <v>36</v>
       </c>
@@ -1588,9 +1588,9 @@
       <c r="H19" s="16"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="58"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="70" t="s">
+      <c r="B20" s="65"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="60" t="s">
         <v>76</v>
       </c>
       <c r="E20" s="10" t="s">
@@ -1603,9 +1603,9 @@
       <c r="H20" s="16"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="58"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="70"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="60"/>
       <c r="E21" s="3" t="s">
         <v>38</v>
       </c>
@@ -1616,9 +1616,9 @@
       <c r="H21" s="16"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="58"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="70"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="60"/>
       <c r="E22" s="4" t="s">
         <v>39</v>
       </c>
@@ -1629,7 +1629,7 @@
       <c r="H22" s="16"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="58"/>
+      <c r="B23" s="65"/>
       <c r="C23" s="3" t="s">
         <v>17</v>
       </c>
@@ -1642,7 +1642,7 @@
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="58"/>
+      <c r="B24" s="65"/>
       <c r="C24" s="4" t="s">
         <v>18</v>
       </c>
@@ -1655,7 +1655,7 @@
       <c r="H24" s="16"/>
     </row>
     <row r="25" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="59"/>
+      <c r="B25" s="66"/>
       <c r="C25" s="22" t="s">
         <v>19</v>
       </c>
@@ -1669,10 +1669,10 @@
     </row>
     <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="67" t="s">
+      <c r="B29" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="55" t="s">
         <v>65</v>
       </c>
       <c r="D29" s="38" t="s">
@@ -1684,8 +1684,8 @@
       <c r="F29" s="35"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="68"/>
-      <c r="C30" s="61"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="56"/>
       <c r="D30" s="39" t="s">
         <v>71</v>
       </c>
@@ -1695,8 +1695,8 @@
       <c r="F30" s="21"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="68"/>
-      <c r="C31" s="61"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="56"/>
       <c r="D31" s="40" t="s">
         <v>73</v>
       </c>
@@ -1706,8 +1706,8 @@
       <c r="F31" s="21"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="68"/>
-      <c r="C32" s="61"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="56"/>
       <c r="D32" s="41" t="s">
         <v>74</v>
       </c>
@@ -1717,8 +1717,8 @@
       <c r="F32" s="21"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="68"/>
-      <c r="C33" s="61"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="56"/>
       <c r="D33" s="42" t="s">
         <v>75</v>
       </c>
@@ -1728,9 +1728,9 @@
       <c r="F33" s="21"/>
     </row>
     <row r="34" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="68"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="66" t="s">
+      <c r="B34" s="58"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="54" t="s">
         <v>76</v>
       </c>
       <c r="E34" s="10" t="s">
@@ -1741,9 +1741,9 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="68"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="66"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="54"/>
       <c r="E35" s="6" t="s">
         <v>38</v>
       </c>
@@ -1752,9 +1752,9 @@
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="68"/>
-      <c r="C36" s="61"/>
-      <c r="D36" s="66"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="54"/>
       <c r="E36" s="7" t="s">
         <v>39</v>
       </c>
@@ -1763,7 +1763,7 @@
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="68"/>
+      <c r="B37" s="58"/>
       <c r="C37" s="43" t="s">
         <v>66</v>
       </c>
@@ -1774,7 +1774,7 @@
       <c r="F37" s="21"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="68"/>
+      <c r="B38" s="58"/>
       <c r="C38" s="39" t="s">
         <v>67</v>
       </c>
@@ -1785,7 +1785,7 @@
       <c r="F38" s="21"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="68"/>
+      <c r="B39" s="58"/>
       <c r="C39" s="40" t="s">
         <v>68</v>
       </c>
@@ -1796,7 +1796,7 @@
       <c r="F39" s="21"/>
     </row>
     <row r="40" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="69"/>
+      <c r="B40" s="59"/>
       <c r="C40" s="44" t="s">
         <v>69</v>
       </c>
@@ -1808,11 +1808,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="C29:C36"/>
-    <mergeCell ref="B29:B40"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="C3:C22"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="F11:F12"/>
@@ -1821,6 +1816,11 @@
     <mergeCell ref="D7:D15"/>
     <mergeCell ref="E10:E12"/>
     <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="C29:C36"/>
+    <mergeCell ref="B29:B40"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="C3:C22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1855,13 +1855,13 @@
     </row>
     <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="55" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -1872,9 +1872,9 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="58"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1883,9 +1883,9 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="58"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1894,8 +1894,8 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="58"/>
-      <c r="C6" s="61"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1905,9 +1905,9 @@
       <c r="F6" s="16"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="58"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="62" t="s">
+      <c r="B7" s="65"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="67" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -1918,9 +1918,9 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="58"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="62"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="67"/>
       <c r="E8" s="9" t="s">
         <v>12</v>
       </c>
@@ -1929,9 +1929,9 @@
       </c>
     </row>
     <row r="9" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="58"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="62"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="67"/>
       <c r="E9" s="25" t="s">
         <v>53</v>
       </c>
@@ -1940,9 +1940,9 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="58"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="62"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="67"/>
       <c r="E10" s="12" t="s">
         <v>21</v>
       </c>
@@ -1951,9 +1951,9 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="58"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="62"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="67"/>
       <c r="E11" s="10" t="s">
         <v>22</v>
       </c>
@@ -1962,9 +1962,9 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="58"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="62"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="67"/>
       <c r="E12" s="3" t="s">
         <v>23</v>
       </c>
@@ -1973,9 +1973,9 @@
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="58"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="65" t="s">
+      <c r="B13" s="65"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="70" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -1986,9 +1986,9 @@
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="58"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="65"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="70"/>
       <c r="E14" s="9" t="s">
         <v>34</v>
       </c>
@@ -1997,9 +1997,9 @@
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="58"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="65"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="70"/>
       <c r="E15" s="8" t="s">
         <v>35</v>
       </c>
@@ -2008,9 +2008,9 @@
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="58"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="65"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="70"/>
       <c r="E16" s="12" t="s">
         <v>36</v>
       </c>
@@ -2019,8 +2019,8 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="58"/>
-      <c r="C17" s="61"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="72" t="s">
         <v>50</v>
       </c>
@@ -2032,9 +2032,9 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="58"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="70"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="60"/>
       <c r="E18" s="3" t="s">
         <v>38</v>
       </c>
@@ -2043,9 +2043,9 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="58"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="70"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="60"/>
       <c r="E19" s="4" t="s">
         <v>39</v>
       </c>
@@ -2054,7 +2054,7 @@
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="58"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="73" t="s">
         <v>49</v>
       </c>
@@ -2067,7 +2067,7 @@
       <c r="F20" s="16"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="58"/>
+      <c r="B21" s="65"/>
       <c r="C21" s="74"/>
       <c r="D21" s="4" t="s">
         <v>18</v>
@@ -2078,7 +2078,7 @@
       <c r="F21" s="16"/>
     </row>
     <row r="22" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="59"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="75"/>
       <c r="D22" s="22" t="s">
         <v>55</v>
@@ -2090,10 +2090,10 @@
     </row>
     <row r="26" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="55" t="s">
         <v>65</v>
       </c>
       <c r="D27" s="38" t="s">
@@ -2105,8 +2105,8 @@
       <c r="F27" s="35"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="68"/>
-      <c r="C28" s="61"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="56"/>
       <c r="D28" s="39" t="s">
         <v>71</v>
       </c>
@@ -2116,8 +2116,8 @@
       <c r="F28" s="21"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="68"/>
-      <c r="C29" s="61"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="56"/>
       <c r="D29" s="40" t="s">
         <v>73</v>
       </c>
@@ -2127,8 +2127,8 @@
       <c r="F29" s="21"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="68"/>
-      <c r="C30" s="61"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="56"/>
       <c r="D30" s="41" t="s">
         <v>74</v>
       </c>
@@ -2138,8 +2138,8 @@
       <c r="F30" s="21"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="68"/>
-      <c r="C31" s="61"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="56"/>
       <c r="D31" s="42" t="s">
         <v>75</v>
       </c>
@@ -2149,9 +2149,9 @@
       <c r="F31" s="21"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="68"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="66" t="s">
+      <c r="B32" s="58"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="54" t="s">
         <v>76</v>
       </c>
       <c r="E32" s="32" t="s">
@@ -2162,9 +2162,9 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="68"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="66"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="54"/>
       <c r="E33" s="33" t="s">
         <v>38</v>
       </c>
@@ -2173,9 +2173,9 @@
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="68"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="66"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="54"/>
       <c r="E34" s="34" t="s">
         <v>39</v>
       </c>
@@ -2184,8 +2184,8 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="68"/>
-      <c r="C35" s="61"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="56"/>
       <c r="D35" s="43" t="s">
         <v>66</v>
       </c>
@@ -2195,8 +2195,8 @@
       <c r="F35" s="21"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="68"/>
-      <c r="C36" s="61"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="56"/>
       <c r="D36" s="39" t="s">
         <v>79</v>
       </c>
@@ -2206,7 +2206,7 @@
       <c r="F36" s="21"/>
     </row>
     <row r="37" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="69"/>
+      <c r="B37" s="59"/>
       <c r="C37" s="51" t="s">
         <v>68</v>
       </c>
@@ -2239,8 +2239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2256,25 +2256,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
     </row>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="55" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="45" t="s">
@@ -2287,9 +2287,9 @@
       <c r="H3" s="15"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="58"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="48" t="s">
         <v>7</v>
       </c>
@@ -2302,9 +2302,9 @@
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="58"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="49" t="s">
         <v>8</v>
       </c>
@@ -2315,8 +2315,8 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="58"/>
-      <c r="C6" s="61"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="48" t="s">
         <v>9</v>
       </c>
@@ -2328,9 +2328,9 @@
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="58"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="62" t="s">
+      <c r="B7" s="65"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="67" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="50" t="s">
@@ -2343,9 +2343,9 @@
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="58"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="62"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="67"/>
       <c r="E8" s="47" t="s">
         <v>12</v>
       </c>
@@ -2356,9 +2356,9 @@
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="58"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="62"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="67"/>
       <c r="E9" s="8" t="s">
         <v>90</v>
       </c>
@@ -2366,15 +2366,15 @@
         <v>1</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H9" s="16"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="58"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="63" t="s">
+      <c r="B10" s="65"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="68" t="s">
         <v>45</v>
       </c>
       <c r="F10" s="46" t="s">
@@ -2388,14 +2388,14 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="58"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="56" t="s">
+      <c r="B11" s="65"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="55" t="s">
+      <c r="G11" s="62" t="s">
         <v>30</v>
       </c>
       <c r="H11" s="18" t="s">
@@ -2403,20 +2403,20 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="58"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="55"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="62"/>
       <c r="H12" s="19" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="58"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="62"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="67"/>
       <c r="E13" s="12" t="s">
         <v>21</v>
       </c>
@@ -2427,9 +2427,9 @@
       <c r="H13" s="16"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="58"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="62"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="67"/>
       <c r="E14" s="46" t="s">
         <v>22</v>
       </c>
@@ -2440,9 +2440,9 @@
       <c r="H14" s="16"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="58"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="62"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="67"/>
       <c r="E15" s="48" t="s">
         <v>23</v>
       </c>
@@ -2453,9 +2453,9 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="58"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="65" t="s">
+      <c r="B16" s="65"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="70" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="50" t="s">
@@ -2465,14 +2465,14 @@
         <v>0</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H16" s="16"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="58"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="65"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="70"/>
       <c r="E17" s="47" t="s">
         <v>34</v>
       </c>
@@ -2483,9 +2483,9 @@
       <c r="H17" s="16"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="58"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="65"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="70"/>
       <c r="E18" s="8" t="s">
         <v>35</v>
       </c>
@@ -2493,14 +2493,14 @@
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H18" s="21"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="58"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="65"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="70"/>
       <c r="E19" s="12" t="s">
         <v>36</v>
       </c>
@@ -2508,14 +2508,14 @@
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H19" s="16"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="58"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="70" t="s">
+      <c r="B20" s="65"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="60" t="s">
         <v>76</v>
       </c>
       <c r="E20" s="46" t="s">
@@ -2528,9 +2528,9 @@
       <c r="H20" s="16"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="58"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="70"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="60"/>
       <c r="E21" s="48" t="s">
         <v>38</v>
       </c>
@@ -2541,9 +2541,9 @@
       <c r="H21" s="16"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="58"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="70"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="60"/>
       <c r="E22" s="49" t="s">
         <v>39</v>
       </c>
@@ -2554,7 +2554,7 @@
       <c r="H22" s="16"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="58"/>
+      <c r="B23" s="65"/>
       <c r="C23" s="48" t="s">
         <v>17</v>
       </c>
@@ -2567,7 +2567,7 @@
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="58"/>
+      <c r="B24" s="65"/>
       <c r="C24" s="49" t="s">
         <v>18</v>
       </c>
@@ -2580,7 +2580,7 @@
       <c r="H24" s="16"/>
     </row>
     <row r="25" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="59"/>
+      <c r="B25" s="66"/>
       <c r="C25" s="22" t="s">
         <v>19</v>
       </c>
@@ -2590,16 +2590,16 @@
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
       <c r="G25" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H25" s="24"/>
     </row>
     <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="67" t="s">
+      <c r="B29" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="55" t="s">
         <v>65</v>
       </c>
       <c r="D29" s="38" t="s">
@@ -2610,13 +2610,13 @@
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H29" s="35"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="68"/>
-      <c r="C30" s="61"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="56"/>
       <c r="D30" s="39" t="s">
         <v>71</v>
       </c>
@@ -2628,8 +2628,8 @@
       <c r="H30" s="21"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="68"/>
-      <c r="C31" s="61"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="56"/>
       <c r="D31" s="40" t="s">
         <v>73</v>
       </c>
@@ -2641,8 +2641,8 @@
       <c r="H31" s="21"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="68"/>
-      <c r="C32" s="61"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="56"/>
       <c r="D32" s="41" t="s">
         <v>74</v>
       </c>
@@ -2654,8 +2654,8 @@
       <c r="H32" s="21"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="68"/>
-      <c r="C33" s="61"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="56"/>
       <c r="D33" s="42" t="s">
         <v>75</v>
       </c>
@@ -2667,9 +2667,9 @@
       <c r="H33" s="21"/>
     </row>
     <row r="34" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="68"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="66" t="s">
+      <c r="B34" s="58"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="54" t="s">
         <v>76</v>
       </c>
       <c r="E34" s="46" t="s">
@@ -2682,9 +2682,9 @@
       <c r="H34" s="21"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="68"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="66"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="54"/>
       <c r="E35" s="48" t="s">
         <v>38</v>
       </c>
@@ -2695,9 +2695,9 @@
       <c r="H35" s="21"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="68"/>
-      <c r="C36" s="61"/>
-      <c r="D36" s="66"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="54"/>
       <c r="E36" s="49" t="s">
         <v>39</v>
       </c>
@@ -2708,7 +2708,7 @@
       <c r="H36" s="21"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="68"/>
+      <c r="B37" s="58"/>
       <c r="C37" s="43" t="s">
         <v>66</v>
       </c>
@@ -2721,7 +2721,7 @@
       <c r="H37" s="21"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="68"/>
+      <c r="B38" s="58"/>
       <c r="C38" s="39" t="s">
         <v>67</v>
       </c>
@@ -2734,7 +2734,7 @@
       <c r="H38" s="21"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="68"/>
+      <c r="B39" s="58"/>
       <c r="C39" s="40" t="s">
         <v>68</v>
       </c>
@@ -2744,12 +2744,12 @@
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
       <c r="G39" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H39" s="21"/>
     </row>
     <row r="40" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="69"/>
+      <c r="B40" s="59"/>
       <c r="C40" s="44" t="s">
         <v>69</v>
       </c>

</xml_diff>